<commit_message>
add parameters of new models
</commit_message>
<xml_diff>
--- a/model parameter.xlsx
+++ b/model parameter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F18891C-2E84-40DD-A6C8-5C360D9DCA42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6568B14B-CC0A-4CC3-82C7-E370AF2CA7E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32415" yWindow="1275" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="43">
   <si>
     <t xml:space="preserve">model </t>
   </si>
@@ -106,13 +106,61 @@
   </si>
   <si>
     <t>unet_9</t>
+  </si>
+  <si>
+    <t>unet_10</t>
+  </si>
+  <si>
+    <t>Average of 4 images</t>
+  </si>
+  <si>
+    <t>unet_11</t>
+  </si>
+  <si>
+    <t>rotation random(-5, 5)</t>
+  </si>
+  <si>
+    <t>unet_12</t>
+  </si>
+  <si>
+    <t>Average of 8 images</t>
+  </si>
+  <si>
+    <t>unet_13</t>
+  </si>
+  <si>
+    <t>unet_14</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>unet_15</t>
+  </si>
+  <si>
+    <t>unet_16</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>unet_17</t>
+  </si>
+  <si>
+    <t>unet_18</t>
+  </si>
+  <si>
+    <t>BinaryCrossentropy</t>
+  </si>
+  <si>
+    <t>HPI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,13 +174,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,17 +210,29 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -433,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,26 +690,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="E8" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>4</v>
       </c>
     </row>
@@ -679,6 +757,230 @@
       </c>
       <c r="G10">
         <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="7">
+        <v>4</v>
+      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="35" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="7">
+        <v>4</v>
+      </c>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+    </row>
+    <row r="39" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="7">
+        <v>4</v>
+      </c>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="N39" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>